<commit_message>
Add new dummy data - add new graphs using this
</commit_message>
<xml_diff>
--- a/DummyData.xlsx
+++ b/DummyData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://impservihub-my.sharepoint.com/personal/nicholas_cassidy_improvementservice_org_uk/Documents/building-standards-dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2CC847A2-85AB-4B13-8367-E67244D14617}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0485EAD-2FF4-4449-980B-06D58D60306C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="35">
   <si>
     <t>Tracking Link</t>
   </si>
@@ -88,52 +88,34 @@
     <t>Quarter 1</t>
   </si>
   <si>
-    <t>Aberdeen City</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Very satisfied</t>
+    <t>1</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>Very good</t>
   </si>
   <si>
-    <t>Agree</t>
-  </si>
-  <si>
-    <t>Satisfied</t>
-  </si>
-  <si>
     <t>Very very good</t>
   </si>
   <si>
     <t>Local Authority?</t>
   </si>
   <si>
-    <t>Strongly agree</t>
-  </si>
-  <si>
     <t>fff</t>
   </si>
   <si>
     <t>ff</t>
   </si>
   <si>
-    <t>Poor</t>
-  </si>
-  <si>
     <t>ffff</t>
   </si>
   <si>
-    <t>Disagree</t>
+    <t>3</t>
   </si>
   <si>
     <t>Quarter 2</t>
@@ -142,16 +124,10 @@
     <t>hhh</t>
   </si>
   <si>
-    <t>Good</t>
-  </si>
-  <si>
     <t>hh</t>
   </si>
   <si>
     <t>jj</t>
-  </si>
-  <si>
-    <t>Very poor</t>
   </si>
 </sst>
 </file>
@@ -500,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W7"/>
+  <dimension ref="A1:W25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -586,68 +562,68 @@
       <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S2" t="s">
         <v>23</v>
       </c>
-      <c r="E2" t="s">
+      <c r="T2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U2" t="s">
         <v>23</v>
       </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>26</v>
-      </c>
-      <c r="R2" t="s">
-        <v>25</v>
-      </c>
-      <c r="S2" t="s">
-        <v>27</v>
-      </c>
-      <c r="T2" t="s">
-        <v>25</v>
-      </c>
-      <c r="U2" t="s">
-        <v>28</v>
-      </c>
       <c r="V2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="W2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:23">
@@ -657,68 +633,68 @@
       <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" t="s">
-        <v>22</v>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
       </c>
       <c r="K3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" t="s">
         <v>24</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>22</v>
+      </c>
+      <c r="R3" t="s">
         <v>26</v>
       </c>
-      <c r="M3" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" t="s">
-        <v>29</v>
-      </c>
-      <c r="O3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R3" t="s">
-        <v>30</v>
-      </c>
       <c r="S3" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="T3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="U3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="V3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="W3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:23">
@@ -728,281 +704,1559 @@
       <c r="B4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
+      <c r="P4">
+        <v>3</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4" t="s">
+        <v>29</v>
+      </c>
+      <c r="S4" t="s">
+        <v>30</v>
+      </c>
+      <c r="T4" t="s">
+        <v>29</v>
+      </c>
+      <c r="U4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" t="s">
-        <v>32</v>
-      </c>
-      <c r="M4" t="s">
-        <v>26</v>
-      </c>
-      <c r="N4" t="s">
-        <v>33</v>
-      </c>
-      <c r="O4" t="s">
-        <v>34</v>
-      </c>
-      <c r="P4" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>26</v>
-      </c>
-      <c r="R4" t="s">
-        <v>35</v>
-      </c>
-      <c r="S4" t="s">
-        <v>36</v>
-      </c>
-      <c r="T4" t="s">
-        <v>35</v>
-      </c>
-      <c r="U4" t="s">
-        <v>28</v>
-      </c>
       <c r="V4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="W4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:23">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="L5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>2</v>
+      </c>
+      <c r="Q5">
+        <v>2</v>
+      </c>
+      <c r="R5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T5" t="s">
+        <v>33</v>
+      </c>
+      <c r="U5" t="s">
         <v>23</v>
       </c>
-      <c r="H5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" t="s">
-        <v>28</v>
-      </c>
-      <c r="L5" t="s">
-        <v>38</v>
-      </c>
-      <c r="M5" t="s">
-        <v>26</v>
-      </c>
-      <c r="N5" t="s">
-        <v>38</v>
-      </c>
-      <c r="O5" t="s">
-        <v>26</v>
-      </c>
-      <c r="P5" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>39</v>
-      </c>
-      <c r="R5" t="s">
-        <v>38</v>
-      </c>
-      <c r="S5" t="s">
-        <v>31</v>
-      </c>
-      <c r="T5" t="s">
-        <v>40</v>
-      </c>
-      <c r="U5" t="s">
-        <v>28</v>
-      </c>
       <c r="V5" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="W5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:23">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" t="s">
-        <v>24</v>
-      </c>
-      <c r="L6" t="s">
-        <v>41</v>
-      </c>
-      <c r="M6" t="s">
-        <v>39</v>
-      </c>
       <c r="N6" t="s">
-        <v>41</v>
-      </c>
-      <c r="O6" t="s">
-        <v>34</v>
-      </c>
-      <c r="P6" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>42</v>
+        <v>34</v>
+      </c>
+      <c r="O6">
+        <v>3</v>
+      </c>
+      <c r="P6">
+        <v>4</v>
+      </c>
+      <c r="Q6">
+        <v>4</v>
       </c>
       <c r="R6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="S6" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="T6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="U6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="V6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="W6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:23">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N7" t="s">
+        <v>34</v>
+      </c>
+      <c r="O7">
+        <v>4</v>
+      </c>
+      <c r="P7">
+        <v>4</v>
+      </c>
+      <c r="Q7">
+        <v>4</v>
+      </c>
+      <c r="R7" t="s">
+        <v>34</v>
+      </c>
+      <c r="S7" t="s">
+        <v>21</v>
+      </c>
+      <c r="T7" t="s">
+        <v>34</v>
+      </c>
+      <c r="U7" t="s">
         <v>23</v>
       </c>
-      <c r="D7" t="s">
+      <c r="V7" t="s">
+        <v>34</v>
+      </c>
+      <c r="W7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>3</v>
+      </c>
+      <c r="L8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" t="s">
+        <v>22</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8" t="s">
+        <v>22</v>
+      </c>
+      <c r="S8" t="s">
         <v>23</v>
       </c>
-      <c r="E7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="T8" t="s">
+        <v>22</v>
+      </c>
+      <c r="U8" t="s">
         <v>23</v>
       </c>
-      <c r="H7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="V8" t="s">
+        <v>22</v>
+      </c>
+      <c r="W8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>4</v>
+      </c>
+      <c r="L9" t="s">
         <v>24</v>
       </c>
-      <c r="L7" t="s">
-        <v>41</v>
-      </c>
-      <c r="M7" t="s">
-        <v>34</v>
-      </c>
-      <c r="N7" t="s">
-        <v>41</v>
-      </c>
-      <c r="O7" t="s">
-        <v>42</v>
-      </c>
-      <c r="P7" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>42</v>
-      </c>
-      <c r="R7" t="s">
-        <v>41</v>
-      </c>
-      <c r="S7" t="s">
+      <c r="M9">
+        <v>4</v>
+      </c>
+      <c r="N9" t="s">
+        <v>25</v>
+      </c>
+      <c r="O9">
+        <v>4</v>
+      </c>
+      <c r="P9">
+        <v>4</v>
+      </c>
+      <c r="Q9">
+        <v>4</v>
+      </c>
+      <c r="R9" t="s">
+        <v>26</v>
+      </c>
+      <c r="S9" t="s">
+        <v>21</v>
+      </c>
+      <c r="T9" t="s">
+        <v>24</v>
+      </c>
+      <c r="U9" t="s">
+        <v>21</v>
+      </c>
+      <c r="V9" t="s">
+        <v>22</v>
+      </c>
+      <c r="W9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>4</v>
+      </c>
+      <c r="L10" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10">
+        <v>3</v>
+      </c>
+      <c r="N10" t="s">
+        <v>28</v>
+      </c>
+      <c r="O10">
+        <v>3</v>
+      </c>
+      <c r="P10">
+        <v>3</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10" t="s">
+        <v>29</v>
+      </c>
+      <c r="S10" t="s">
+        <v>30</v>
+      </c>
+      <c r="T10" t="s">
+        <v>29</v>
+      </c>
+      <c r="U10">
+        <v>4</v>
+      </c>
+      <c r="V10" t="s">
+        <v>29</v>
+      </c>
+      <c r="W10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
+      <c r="A11" t="s">
         <v>31</v>
       </c>
-      <c r="T7" t="s">
-        <v>41</v>
-      </c>
-      <c r="U7" t="s">
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>3</v>
+      </c>
+      <c r="L11" t="s">
+        <v>32</v>
+      </c>
+      <c r="M11">
+        <v>3</v>
+      </c>
+      <c r="N11" t="s">
+        <v>32</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>2</v>
+      </c>
+      <c r="Q11">
+        <v>2</v>
+      </c>
+      <c r="R11" t="s">
+        <v>32</v>
+      </c>
+      <c r="S11" t="s">
+        <v>21</v>
+      </c>
+      <c r="T11" t="s">
+        <v>33</v>
+      </c>
+      <c r="U11">
+        <v>3</v>
+      </c>
+      <c r="V11" t="s">
+        <v>33</v>
+      </c>
+      <c r="W11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>3</v>
+      </c>
+      <c r="L12" t="s">
+        <v>34</v>
+      </c>
+      <c r="M12">
+        <v>3</v>
+      </c>
+      <c r="N12" t="s">
+        <v>34</v>
+      </c>
+      <c r="O12">
+        <v>3</v>
+      </c>
+      <c r="P12">
+        <v>4</v>
+      </c>
+      <c r="Q12">
+        <v>4</v>
+      </c>
+      <c r="R12" t="s">
+        <v>34</v>
+      </c>
+      <c r="S12" t="s">
+        <v>21</v>
+      </c>
+      <c r="T12" t="s">
+        <v>34</v>
+      </c>
+      <c r="U12" t="s">
+        <v>21</v>
+      </c>
+      <c r="V12" t="s">
+        <v>34</v>
+      </c>
+      <c r="W12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13" t="s">
+        <v>34</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13" t="s">
+        <v>34</v>
+      </c>
+      <c r="O13">
+        <v>4</v>
+      </c>
+      <c r="P13">
+        <v>4</v>
+      </c>
+      <c r="Q13">
+        <v>4</v>
+      </c>
+      <c r="R13" t="s">
+        <v>34</v>
+      </c>
+      <c r="S13" t="s">
+        <v>21</v>
+      </c>
+      <c r="T13" t="s">
+        <v>34</v>
+      </c>
+      <c r="U13" t="s">
+        <v>23</v>
+      </c>
+      <c r="V13" t="s">
+        <v>34</v>
+      </c>
+      <c r="W13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" t="s">
+        <v>21</v>
+      </c>
+      <c r="N14" t="s">
+        <v>22</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="R14" t="s">
+        <v>22</v>
+      </c>
+      <c r="S14" t="s">
+        <v>23</v>
+      </c>
+      <c r="T14" t="s">
+        <v>22</v>
+      </c>
+      <c r="U14" t="s">
+        <v>23</v>
+      </c>
+      <c r="V14" t="s">
+        <v>22</v>
+      </c>
+      <c r="W14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15" t="s">
+        <v>24</v>
+      </c>
+      <c r="M15" t="s">
+        <v>21</v>
+      </c>
+      <c r="N15" t="s">
+        <v>25</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>22</v>
+      </c>
+      <c r="R15" t="s">
+        <v>26</v>
+      </c>
+      <c r="S15" t="s">
+        <v>21</v>
+      </c>
+      <c r="T15" t="s">
+        <v>24</v>
+      </c>
+      <c r="U15" t="s">
+        <v>21</v>
+      </c>
+      <c r="V15" t="s">
+        <v>22</v>
+      </c>
+      <c r="W15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" t="s">
+        <v>27</v>
+      </c>
+      <c r="M16" t="s">
+        <v>21</v>
+      </c>
+      <c r="N16" t="s">
         <v>28</v>
       </c>
-      <c r="V7" t="s">
-        <v>41</v>
-      </c>
-      <c r="W7" t="s">
-        <v>41</v>
+      <c r="O16">
+        <v>3</v>
+      </c>
+      <c r="P16">
+        <v>3</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="R16" t="s">
+        <v>29</v>
+      </c>
+      <c r="S16" t="s">
+        <v>30</v>
+      </c>
+      <c r="T16" t="s">
+        <v>29</v>
+      </c>
+      <c r="U16" t="s">
+        <v>23</v>
+      </c>
+      <c r="V16" t="s">
+        <v>29</v>
+      </c>
+      <c r="W16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17" t="s">
+        <v>23</v>
+      </c>
+      <c r="L17" t="s">
+        <v>32</v>
+      </c>
+      <c r="M17" t="s">
+        <v>21</v>
+      </c>
+      <c r="N17" t="s">
+        <v>32</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <v>2</v>
+      </c>
+      <c r="Q17">
+        <v>2</v>
+      </c>
+      <c r="R17" t="s">
+        <v>32</v>
+      </c>
+      <c r="S17" t="s">
+        <v>21</v>
+      </c>
+      <c r="T17" t="s">
+        <v>33</v>
+      </c>
+      <c r="U17" t="s">
+        <v>23</v>
+      </c>
+      <c r="V17" t="s">
+        <v>33</v>
+      </c>
+      <c r="W17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18" t="s">
+        <v>34</v>
+      </c>
+      <c r="M18" t="s">
+        <v>23</v>
+      </c>
+      <c r="N18" t="s">
+        <v>34</v>
+      </c>
+      <c r="O18">
+        <v>3</v>
+      </c>
+      <c r="P18">
+        <v>4</v>
+      </c>
+      <c r="Q18">
+        <v>4</v>
+      </c>
+      <c r="R18" t="s">
+        <v>34</v>
+      </c>
+      <c r="S18" t="s">
+        <v>21</v>
+      </c>
+      <c r="T18" t="s">
+        <v>34</v>
+      </c>
+      <c r="U18" t="s">
+        <v>21</v>
+      </c>
+      <c r="V18" t="s">
+        <v>34</v>
+      </c>
+      <c r="W18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" t="s">
+        <v>34</v>
+      </c>
+      <c r="M19" t="s">
+        <v>30</v>
+      </c>
+      <c r="N19" t="s">
+        <v>34</v>
+      </c>
+      <c r="O19">
+        <v>4</v>
+      </c>
+      <c r="P19">
+        <v>4</v>
+      </c>
+      <c r="Q19">
+        <v>4</v>
+      </c>
+      <c r="R19" t="s">
+        <v>34</v>
+      </c>
+      <c r="S19" t="s">
+        <v>21</v>
+      </c>
+      <c r="T19" t="s">
+        <v>34</v>
+      </c>
+      <c r="U19" t="s">
+        <v>23</v>
+      </c>
+      <c r="V19" t="s">
+        <v>34</v>
+      </c>
+      <c r="W19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>3</v>
+      </c>
+      <c r="L20" t="s">
+        <v>22</v>
+      </c>
+      <c r="M20" t="s">
+        <v>21</v>
+      </c>
+      <c r="N20" t="s">
+        <v>22</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>1</v>
+      </c>
+      <c r="R20" t="s">
+        <v>22</v>
+      </c>
+      <c r="S20" t="s">
+        <v>23</v>
+      </c>
+      <c r="T20" t="s">
+        <v>22</v>
+      </c>
+      <c r="U20" t="s">
+        <v>23</v>
+      </c>
+      <c r="V20" t="s">
+        <v>22</v>
+      </c>
+      <c r="W20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>4</v>
+      </c>
+      <c r="L21" t="s">
+        <v>24</v>
+      </c>
+      <c r="M21">
+        <v>4</v>
+      </c>
+      <c r="N21" t="s">
+        <v>25</v>
+      </c>
+      <c r="O21">
+        <v>4</v>
+      </c>
+      <c r="P21">
+        <v>4</v>
+      </c>
+      <c r="Q21">
+        <v>4</v>
+      </c>
+      <c r="R21" t="s">
+        <v>26</v>
+      </c>
+      <c r="S21" t="s">
+        <v>21</v>
+      </c>
+      <c r="T21" t="s">
+        <v>24</v>
+      </c>
+      <c r="U21" t="s">
+        <v>21</v>
+      </c>
+      <c r="V21" t="s">
+        <v>22</v>
+      </c>
+      <c r="W21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>4</v>
+      </c>
+      <c r="L22" t="s">
+        <v>27</v>
+      </c>
+      <c r="M22">
+        <v>3</v>
+      </c>
+      <c r="N22" t="s">
+        <v>28</v>
+      </c>
+      <c r="O22">
+        <v>3</v>
+      </c>
+      <c r="P22">
+        <v>3</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22" t="s">
+        <v>29</v>
+      </c>
+      <c r="S22" t="s">
+        <v>30</v>
+      </c>
+      <c r="T22" t="s">
+        <v>29</v>
+      </c>
+      <c r="U22">
+        <v>4</v>
+      </c>
+      <c r="V22" t="s">
+        <v>29</v>
+      </c>
+      <c r="W22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>3</v>
+      </c>
+      <c r="L23" t="s">
+        <v>32</v>
+      </c>
+      <c r="M23">
+        <v>3</v>
+      </c>
+      <c r="N23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="P23">
+        <v>2</v>
+      </c>
+      <c r="Q23">
+        <v>2</v>
+      </c>
+      <c r="R23" t="s">
+        <v>32</v>
+      </c>
+      <c r="S23" t="s">
+        <v>21</v>
+      </c>
+      <c r="T23" t="s">
+        <v>33</v>
+      </c>
+      <c r="U23">
+        <v>3</v>
+      </c>
+      <c r="V23" t="s">
+        <v>33</v>
+      </c>
+      <c r="W23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>3</v>
+      </c>
+      <c r="L24" t="s">
+        <v>34</v>
+      </c>
+      <c r="M24">
+        <v>3</v>
+      </c>
+      <c r="N24" t="s">
+        <v>34</v>
+      </c>
+      <c r="O24">
+        <v>3</v>
+      </c>
+      <c r="P24">
+        <v>4</v>
+      </c>
+      <c r="Q24">
+        <v>4</v>
+      </c>
+      <c r="R24" t="s">
+        <v>34</v>
+      </c>
+      <c r="S24" t="s">
+        <v>21</v>
+      </c>
+      <c r="T24" t="s">
+        <v>34</v>
+      </c>
+      <c r="U24" t="s">
+        <v>21</v>
+      </c>
+      <c r="V24" t="s">
+        <v>34</v>
+      </c>
+      <c r="W24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25" t="s">
+        <v>34</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25" t="s">
+        <v>34</v>
+      </c>
+      <c r="O25">
+        <v>4</v>
+      </c>
+      <c r="P25">
+        <v>4</v>
+      </c>
+      <c r="Q25">
+        <v>4</v>
+      </c>
+      <c r="R25" t="s">
+        <v>34</v>
+      </c>
+      <c r="S25" t="s">
+        <v>21</v>
+      </c>
+      <c r="T25" t="s">
+        <v>34</v>
+      </c>
+      <c r="U25" t="s">
+        <v>23</v>
+      </c>
+      <c r="V25" t="s">
+        <v>34</v>
+      </c>
+      <c r="W25" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1250,7 +2504,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90DD76C3-DF31-4720-BD5D-13CD8E110329}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96F575C8-B90C-497F-AAE8-0422E3737517}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -1269,7 +2523,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D597A62-552B-4957-BD07-8C21F09A8D51}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0E30D80-A26F-4E4D-9CBA-B8BAC83AC309}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
@@ -1277,7 +2531,7 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAEB98E7-BD4C-43DE-AFC6-9AF409A35934}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{273608FC-09B2-466F-989B-E66C1F12EE0E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>

</xml_diff>

<commit_message>
Added 1 response from another council to test graphs
</commit_message>
<xml_diff>
--- a/DummyData.xlsx
+++ b/DummyData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://impservihub-my.sharepoint.com/personal/nicholas_cassidy_improvementservice_org_uk/Documents/building-standards-dashboard/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\connachan.cara\Documents\building-standards-dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0485EAD-2FF4-4449-980B-06D58D60306C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C28562-BBC1-4B19-84B8-C139F553BB88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="33">
   <si>
     <t>Tracking Link</t>
   </si>
@@ -94,9 +94,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>Very good</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
   </si>
   <si>
     <t>ffff</t>
-  </si>
-  <si>
-    <t>3</t>
   </si>
   <si>
     <t>Quarter 2</t>
@@ -476,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W25"/>
+  <dimension ref="A1:W26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
+      <selection activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -586,14 +580,14 @@
       <c r="J2">
         <v>0</v>
       </c>
-      <c r="K2" t="s">
-        <v>21</v>
+      <c r="K2">
+        <v>1</v>
       </c>
       <c r="L2" t="s">
         <v>22</v>
       </c>
-      <c r="M2" t="s">
-        <v>21</v>
+      <c r="M2">
+        <v>1</v>
       </c>
       <c r="N2" t="s">
         <v>22</v>
@@ -610,14 +604,14 @@
       <c r="R2" t="s">
         <v>22</v>
       </c>
-      <c r="S2" t="s">
-        <v>23</v>
+      <c r="S2">
+        <v>2</v>
       </c>
       <c r="T2" t="s">
         <v>22</v>
       </c>
-      <c r="U2" t="s">
-        <v>23</v>
+      <c r="U2">
+        <v>2</v>
       </c>
       <c r="V2" t="s">
         <v>22</v>
@@ -657,38 +651,38 @@
       <c r="J3">
         <v>0</v>
       </c>
-      <c r="K3" t="s">
-        <v>21</v>
+      <c r="K3">
+        <v>1</v>
       </c>
       <c r="L3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
         <v>24</v>
       </c>
-      <c r="M3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>22</v>
+      </c>
+      <c r="R3" t="s">
         <v>25</v>
       </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
-      <c r="P3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>22</v>
-      </c>
-      <c r="R3" t="s">
-        <v>26</v>
-      </c>
-      <c r="S3" t="s">
-        <v>21</v>
+      <c r="S3">
+        <v>1</v>
       </c>
       <c r="T3" t="s">
-        <v>24</v>
-      </c>
-      <c r="U3" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
       </c>
       <c r="V3" t="s">
         <v>22</v>
@@ -728,41 +722,41 @@
       <c r="J4">
         <v>0</v>
       </c>
-      <c r="K4" t="s">
-        <v>21</v>
+      <c r="K4">
+        <v>1</v>
       </c>
       <c r="L4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4" t="s">
         <v>27</v>
       </c>
-      <c r="M4" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="O4">
+        <v>3</v>
+      </c>
+      <c r="P4">
+        <v>3</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4" t="s">
         <v>28</v>
       </c>
-      <c r="O4">
-        <v>3</v>
-      </c>
-      <c r="P4">
-        <v>3</v>
-      </c>
-      <c r="Q4">
-        <v>1</v>
-      </c>
-      <c r="R4" t="s">
-        <v>29</v>
-      </c>
-      <c r="S4" t="s">
-        <v>30</v>
+      <c r="S4">
+        <v>3</v>
       </c>
       <c r="T4" t="s">
-        <v>29</v>
-      </c>
-      <c r="U4" t="s">
-        <v>23</v>
+        <v>28</v>
+      </c>
+      <c r="U4">
+        <v>2</v>
       </c>
       <c r="V4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W4" t="s">
         <v>22</v>
@@ -770,7 +764,7 @@
     </row>
     <row r="5" spans="1:23">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -799,17 +793,17 @@
       <c r="J5">
         <v>0</v>
       </c>
-      <c r="K5" t="s">
-        <v>23</v>
+      <c r="K5">
+        <v>2</v>
       </c>
       <c r="L5" t="s">
-        <v>32</v>
-      </c>
-      <c r="M5" t="s">
-        <v>21</v>
+        <v>30</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
       </c>
       <c r="N5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="O5">
         <v>1</v>
@@ -821,19 +815,19 @@
         <v>2</v>
       </c>
       <c r="R5" t="s">
-        <v>32</v>
-      </c>
-      <c r="S5" t="s">
-        <v>21</v>
+        <v>30</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
       </c>
       <c r="T5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U5" t="s">
-        <v>23</v>
+        <v>31</v>
+      </c>
+      <c r="U5">
+        <v>2</v>
       </c>
       <c r="V5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="W5" t="s">
         <v>22</v>
@@ -841,7 +835,7 @@
     </row>
     <row r="6" spans="1:23">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
@@ -870,17 +864,17 @@
       <c r="J6">
         <v>0</v>
       </c>
-      <c r="K6" t="s">
-        <v>21</v>
+      <c r="K6">
+        <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M6" t="s">
-        <v>23</v>
+        <v>32</v>
+      </c>
+      <c r="M6">
+        <v>2</v>
       </c>
       <c r="N6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="O6">
         <v>3</v>
@@ -892,27 +886,27 @@
         <v>4</v>
       </c>
       <c r="R6" t="s">
-        <v>34</v>
-      </c>
-      <c r="S6" t="s">
-        <v>21</v>
+        <v>32</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
       </c>
       <c r="T6" t="s">
-        <v>34</v>
-      </c>
-      <c r="U6" t="s">
-        <v>21</v>
+        <v>32</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
       </c>
       <c r="V6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="W6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:23">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
@@ -941,17 +935,17 @@
       <c r="J7">
         <v>0</v>
       </c>
-      <c r="K7" t="s">
-        <v>21</v>
+      <c r="K7">
+        <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>34</v>
-      </c>
-      <c r="M7" t="s">
-        <v>30</v>
+        <v>32</v>
+      </c>
+      <c r="M7">
+        <v>3</v>
       </c>
       <c r="N7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="O7">
         <v>4</v>
@@ -963,22 +957,22 @@
         <v>4</v>
       </c>
       <c r="R7" t="s">
-        <v>34</v>
-      </c>
-      <c r="S7" t="s">
-        <v>21</v>
+        <v>32</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
       </c>
       <c r="T7" t="s">
-        <v>34</v>
-      </c>
-      <c r="U7" t="s">
-        <v>23</v>
+        <v>32</v>
+      </c>
+      <c r="U7">
+        <v>2</v>
       </c>
       <c r="V7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="W7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:23">
@@ -1018,8 +1012,8 @@
       <c r="L8" t="s">
         <v>22</v>
       </c>
-      <c r="M8" t="s">
-        <v>21</v>
+      <c r="M8">
+        <v>1</v>
       </c>
       <c r="N8" t="s">
         <v>22</v>
@@ -1036,14 +1030,14 @@
       <c r="R8" t="s">
         <v>22</v>
       </c>
-      <c r="S8" t="s">
-        <v>23</v>
+      <c r="S8">
+        <v>2</v>
       </c>
       <c r="T8" t="s">
         <v>22</v>
       </c>
-      <c r="U8" t="s">
-        <v>23</v>
+      <c r="U8">
+        <v>2</v>
       </c>
       <c r="V8" t="s">
         <v>22</v>
@@ -1087,34 +1081,34 @@
         <v>4</v>
       </c>
       <c r="L9" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9">
+        <v>4</v>
+      </c>
+      <c r="N9" t="s">
         <v>24</v>
       </c>
-      <c r="M9">
-        <v>4</v>
-      </c>
-      <c r="N9" t="s">
+      <c r="O9">
+        <v>4</v>
+      </c>
+      <c r="P9">
+        <v>4</v>
+      </c>
+      <c r="Q9">
+        <v>4</v>
+      </c>
+      <c r="R9" t="s">
         <v>25</v>
       </c>
-      <c r="O9">
-        <v>4</v>
-      </c>
-      <c r="P9">
-        <v>4</v>
-      </c>
-      <c r="Q9">
-        <v>4</v>
-      </c>
-      <c r="R9" t="s">
-        <v>26</v>
-      </c>
-      <c r="S9" t="s">
-        <v>21</v>
+      <c r="S9">
+        <v>1</v>
       </c>
       <c r="T9" t="s">
-        <v>24</v>
-      </c>
-      <c r="U9" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="U9">
+        <v>1</v>
       </c>
       <c r="V9" t="s">
         <v>22</v>
@@ -1158,37 +1152,37 @@
         <v>4</v>
       </c>
       <c r="L10" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10">
+        <v>3</v>
+      </c>
+      <c r="N10" t="s">
         <v>27</v>
       </c>
-      <c r="M10">
-        <v>3</v>
-      </c>
-      <c r="N10" t="s">
+      <c r="O10">
+        <v>3</v>
+      </c>
+      <c r="P10">
+        <v>3</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10" t="s">
         <v>28</v>
       </c>
-      <c r="O10">
-        <v>3</v>
-      </c>
-      <c r="P10">
-        <v>3</v>
-      </c>
-      <c r="Q10">
-        <v>1</v>
-      </c>
-      <c r="R10" t="s">
-        <v>29</v>
-      </c>
-      <c r="S10" t="s">
-        <v>30</v>
+      <c r="S10">
+        <v>3</v>
       </c>
       <c r="T10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="U10">
         <v>4</v>
       </c>
       <c r="V10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W10" t="s">
         <v>22</v>
@@ -1196,7 +1190,7 @@
     </row>
     <row r="11" spans="1:23">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
@@ -1229,13 +1223,13 @@
         <v>3</v>
       </c>
       <c r="L11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M11">
         <v>3</v>
       </c>
       <c r="N11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="O11">
         <v>1</v>
@@ -1247,19 +1241,19 @@
         <v>2</v>
       </c>
       <c r="R11" t="s">
-        <v>32</v>
-      </c>
-      <c r="S11" t="s">
-        <v>21</v>
+        <v>30</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
       </c>
       <c r="T11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="U11">
         <v>3</v>
       </c>
       <c r="V11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="W11" t="s">
         <v>22</v>
@@ -1267,7 +1261,7 @@
     </row>
     <row r="12" spans="1:23">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
@@ -1300,13 +1294,13 @@
         <v>3</v>
       </c>
       <c r="L12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M12">
         <v>3</v>
       </c>
       <c r="N12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="O12">
         <v>3</v>
@@ -1318,27 +1312,27 @@
         <v>4</v>
       </c>
       <c r="R12" t="s">
-        <v>34</v>
-      </c>
-      <c r="S12" t="s">
-        <v>21</v>
+        <v>32</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
       </c>
       <c r="T12" t="s">
-        <v>34</v>
-      </c>
-      <c r="U12" t="s">
-        <v>21</v>
+        <v>32</v>
+      </c>
+      <c r="U12">
+        <v>1</v>
       </c>
       <c r="V12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="W12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:23">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
         <v>21</v>
@@ -1371,13 +1365,13 @@
         <v>1</v>
       </c>
       <c r="L13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M13">
         <v>1</v>
       </c>
       <c r="N13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="O13">
         <v>4</v>
@@ -1389,22 +1383,22 @@
         <v>4</v>
       </c>
       <c r="R13" t="s">
-        <v>34</v>
-      </c>
-      <c r="S13" t="s">
-        <v>21</v>
+        <v>32</v>
+      </c>
+      <c r="S13">
+        <v>1</v>
       </c>
       <c r="T13" t="s">
-        <v>34</v>
-      </c>
-      <c r="U13" t="s">
-        <v>23</v>
+        <v>32</v>
+      </c>
+      <c r="U13">
+        <v>2</v>
       </c>
       <c r="V13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="W13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:23">
@@ -1438,14 +1432,14 @@
       <c r="J14">
         <v>0</v>
       </c>
-      <c r="K14" t="s">
-        <v>21</v>
+      <c r="K14">
+        <v>1</v>
       </c>
       <c r="L14" t="s">
         <v>22</v>
       </c>
-      <c r="M14" t="s">
-        <v>21</v>
+      <c r="M14">
+        <v>1</v>
       </c>
       <c r="N14" t="s">
         <v>22</v>
@@ -1462,14 +1456,14 @@
       <c r="R14" t="s">
         <v>22</v>
       </c>
-      <c r="S14" t="s">
-        <v>23</v>
+      <c r="S14">
+        <v>2</v>
       </c>
       <c r="T14" t="s">
         <v>22</v>
       </c>
-      <c r="U14" t="s">
-        <v>23</v>
+      <c r="U14">
+        <v>2</v>
       </c>
       <c r="V14" t="s">
         <v>22</v>
@@ -1509,38 +1503,38 @@
       <c r="J15">
         <v>0</v>
       </c>
-      <c r="K15" t="s">
-        <v>21</v>
+      <c r="K15">
+        <v>1</v>
       </c>
       <c r="L15" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15" t="s">
         <v>24</v>
       </c>
-      <c r="M15" t="s">
-        <v>21</v>
-      </c>
-      <c r="N15" t="s">
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>22</v>
+      </c>
+      <c r="R15" t="s">
         <v>25</v>
       </c>
-      <c r="O15">
-        <v>1</v>
-      </c>
-      <c r="P15" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>22</v>
-      </c>
-      <c r="R15" t="s">
-        <v>26</v>
-      </c>
-      <c r="S15" t="s">
-        <v>21</v>
+      <c r="S15">
+        <v>1</v>
       </c>
       <c r="T15" t="s">
-        <v>24</v>
-      </c>
-      <c r="U15" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="U15">
+        <v>1</v>
       </c>
       <c r="V15" t="s">
         <v>22</v>
@@ -1580,41 +1574,41 @@
       <c r="J16">
         <v>0</v>
       </c>
-      <c r="K16" t="s">
-        <v>21</v>
+      <c r="K16">
+        <v>1</v>
       </c>
       <c r="L16" t="s">
+        <v>26</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16" t="s">
         <v>27</v>
       </c>
-      <c r="M16" t="s">
-        <v>21</v>
-      </c>
-      <c r="N16" t="s">
+      <c r="O16">
+        <v>3</v>
+      </c>
+      <c r="P16">
+        <v>3</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="R16" t="s">
         <v>28</v>
       </c>
-      <c r="O16">
-        <v>3</v>
-      </c>
-      <c r="P16">
-        <v>3</v>
-      </c>
-      <c r="Q16">
-        <v>1</v>
-      </c>
-      <c r="R16" t="s">
-        <v>29</v>
-      </c>
-      <c r="S16" t="s">
-        <v>30</v>
+      <c r="S16">
+        <v>3</v>
       </c>
       <c r="T16" t="s">
-        <v>29</v>
-      </c>
-      <c r="U16" t="s">
-        <v>23</v>
+        <v>28</v>
+      </c>
+      <c r="U16">
+        <v>2</v>
       </c>
       <c r="V16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W16" t="s">
         <v>22</v>
@@ -1622,7 +1616,7 @@
     </row>
     <row r="17" spans="1:23">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
         <v>21</v>
@@ -1651,17 +1645,17 @@
       <c r="J17">
         <v>0</v>
       </c>
-      <c r="K17" t="s">
-        <v>23</v>
+      <c r="K17">
+        <v>2</v>
       </c>
       <c r="L17" t="s">
-        <v>32</v>
-      </c>
-      <c r="M17" t="s">
-        <v>21</v>
+        <v>30</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
       </c>
       <c r="N17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="O17">
         <v>1</v>
@@ -1673,19 +1667,19 @@
         <v>2</v>
       </c>
       <c r="R17" t="s">
-        <v>32</v>
-      </c>
-      <c r="S17" t="s">
-        <v>21</v>
+        <v>30</v>
+      </c>
+      <c r="S17">
+        <v>1</v>
       </c>
       <c r="T17" t="s">
-        <v>33</v>
-      </c>
-      <c r="U17" t="s">
-        <v>23</v>
+        <v>31</v>
+      </c>
+      <c r="U17">
+        <v>2</v>
       </c>
       <c r="V17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="W17" t="s">
         <v>22</v>
@@ -1693,7 +1687,7 @@
     </row>
     <row r="18" spans="1:23">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
         <v>21</v>
@@ -1722,17 +1716,17 @@
       <c r="J18">
         <v>0</v>
       </c>
-      <c r="K18" t="s">
-        <v>21</v>
+      <c r="K18">
+        <v>1</v>
       </c>
       <c r="L18" t="s">
-        <v>34</v>
-      </c>
-      <c r="M18" t="s">
-        <v>23</v>
+        <v>32</v>
+      </c>
+      <c r="M18">
+        <v>2</v>
       </c>
       <c r="N18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="O18">
         <v>3</v>
@@ -1744,27 +1738,27 @@
         <v>4</v>
       </c>
       <c r="R18" t="s">
-        <v>34</v>
-      </c>
-      <c r="S18" t="s">
-        <v>21</v>
+        <v>32</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
       </c>
       <c r="T18" t="s">
-        <v>34</v>
-      </c>
-      <c r="U18" t="s">
-        <v>21</v>
+        <v>32</v>
+      </c>
+      <c r="U18">
+        <v>1</v>
       </c>
       <c r="V18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="W18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:23">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s">
         <v>21</v>
@@ -1793,17 +1787,17 @@
       <c r="J19">
         <v>0</v>
       </c>
-      <c r="K19" t="s">
-        <v>21</v>
+      <c r="K19">
+        <v>1</v>
       </c>
       <c r="L19" t="s">
-        <v>34</v>
-      </c>
-      <c r="M19" t="s">
-        <v>30</v>
+        <v>32</v>
+      </c>
+      <c r="M19">
+        <v>3</v>
       </c>
       <c r="N19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="O19">
         <v>4</v>
@@ -1815,22 +1809,22 @@
         <v>4</v>
       </c>
       <c r="R19" t="s">
-        <v>34</v>
-      </c>
-      <c r="S19" t="s">
-        <v>21</v>
+        <v>32</v>
+      </c>
+      <c r="S19">
+        <v>1</v>
       </c>
       <c r="T19" t="s">
-        <v>34</v>
-      </c>
-      <c r="U19" t="s">
-        <v>23</v>
+        <v>32</v>
+      </c>
+      <c r="U19">
+        <v>2</v>
       </c>
       <c r="V19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="W19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:23">
@@ -1870,8 +1864,8 @@
       <c r="L20" t="s">
         <v>22</v>
       </c>
-      <c r="M20" t="s">
-        <v>21</v>
+      <c r="M20">
+        <v>1</v>
       </c>
       <c r="N20" t="s">
         <v>22</v>
@@ -1888,14 +1882,14 @@
       <c r="R20" t="s">
         <v>22</v>
       </c>
-      <c r="S20" t="s">
-        <v>23</v>
+      <c r="S20">
+        <v>2</v>
       </c>
       <c r="T20" t="s">
         <v>22</v>
       </c>
-      <c r="U20" t="s">
-        <v>23</v>
+      <c r="U20">
+        <v>2</v>
       </c>
       <c r="V20" t="s">
         <v>22</v>
@@ -1939,34 +1933,34 @@
         <v>4</v>
       </c>
       <c r="L21" t="s">
+        <v>23</v>
+      </c>
+      <c r="M21">
+        <v>4</v>
+      </c>
+      <c r="N21" t="s">
         <v>24</v>
       </c>
-      <c r="M21">
-        <v>4</v>
-      </c>
-      <c r="N21" t="s">
+      <c r="O21">
+        <v>4</v>
+      </c>
+      <c r="P21">
+        <v>4</v>
+      </c>
+      <c r="Q21">
+        <v>4</v>
+      </c>
+      <c r="R21" t="s">
         <v>25</v>
       </c>
-      <c r="O21">
-        <v>4</v>
-      </c>
-      <c r="P21">
-        <v>4</v>
-      </c>
-      <c r="Q21">
-        <v>4</v>
-      </c>
-      <c r="R21" t="s">
-        <v>26</v>
-      </c>
-      <c r="S21" t="s">
-        <v>21</v>
+      <c r="S21">
+        <v>1</v>
       </c>
       <c r="T21" t="s">
-        <v>24</v>
-      </c>
-      <c r="U21" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="U21">
+        <v>1</v>
       </c>
       <c r="V21" t="s">
         <v>22</v>
@@ -2010,37 +2004,37 @@
         <v>4</v>
       </c>
       <c r="L22" t="s">
+        <v>26</v>
+      </c>
+      <c r="M22">
+        <v>3</v>
+      </c>
+      <c r="N22" t="s">
         <v>27</v>
       </c>
-      <c r="M22">
-        <v>3</v>
-      </c>
-      <c r="N22" t="s">
+      <c r="O22">
+        <v>3</v>
+      </c>
+      <c r="P22">
+        <v>3</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22" t="s">
         <v>28</v>
       </c>
-      <c r="O22">
-        <v>3</v>
-      </c>
-      <c r="P22">
-        <v>3</v>
-      </c>
-      <c r="Q22">
-        <v>1</v>
-      </c>
-      <c r="R22" t="s">
-        <v>29</v>
-      </c>
-      <c r="S22" t="s">
-        <v>30</v>
+      <c r="S22">
+        <v>3</v>
       </c>
       <c r="T22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="U22">
         <v>4</v>
       </c>
       <c r="V22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W22" t="s">
         <v>22</v>
@@ -2048,7 +2042,7 @@
     </row>
     <row r="23" spans="1:23">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
         <v>21</v>
@@ -2081,13 +2075,13 @@
         <v>3</v>
       </c>
       <c r="L23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M23">
         <v>3</v>
       </c>
       <c r="N23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="O23">
         <v>1</v>
@@ -2099,19 +2093,19 @@
         <v>2</v>
       </c>
       <c r="R23" t="s">
-        <v>32</v>
-      </c>
-      <c r="S23" t="s">
-        <v>21</v>
+        <v>30</v>
+      </c>
+      <c r="S23">
+        <v>1</v>
       </c>
       <c r="T23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="U23">
         <v>3</v>
       </c>
       <c r="V23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="W23" t="s">
         <v>22</v>
@@ -2119,7 +2113,7 @@
     </row>
     <row r="24" spans="1:23">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s">
         <v>21</v>
@@ -2152,13 +2146,13 @@
         <v>3</v>
       </c>
       <c r="L24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M24">
         <v>3</v>
       </c>
       <c r="N24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="O24">
         <v>3</v>
@@ -2170,27 +2164,27 @@
         <v>4</v>
       </c>
       <c r="R24" t="s">
-        <v>34</v>
-      </c>
-      <c r="S24" t="s">
-        <v>21</v>
+        <v>32</v>
+      </c>
+      <c r="S24">
+        <v>1</v>
       </c>
       <c r="T24" t="s">
-        <v>34</v>
-      </c>
-      <c r="U24" t="s">
-        <v>21</v>
+        <v>32</v>
+      </c>
+      <c r="U24">
+        <v>1</v>
       </c>
       <c r="V24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="W24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:23">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
         <v>21</v>
@@ -2223,13 +2217,13 @@
         <v>1</v>
       </c>
       <c r="L25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M25">
         <v>1</v>
       </c>
       <c r="N25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="O25">
         <v>4</v>
@@ -2241,22 +2235,93 @@
         <v>4</v>
       </c>
       <c r="R25" t="s">
-        <v>34</v>
-      </c>
-      <c r="S25" t="s">
-        <v>21</v>
+        <v>32</v>
+      </c>
+      <c r="S25">
+        <v>1</v>
       </c>
       <c r="T25" t="s">
-        <v>34</v>
-      </c>
-      <c r="U25" t="s">
-        <v>23</v>
+        <v>32</v>
+      </c>
+      <c r="U25">
+        <v>2</v>
       </c>
       <c r="V25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="W25" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23">
+      <c r="A26" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>3</v>
+      </c>
+      <c r="L26" t="s">
+        <v>22</v>
+      </c>
+      <c r="M26">
+        <v>1</v>
+      </c>
+      <c r="N26" t="s">
+        <v>22</v>
+      </c>
+      <c r="O26">
+        <v>4</v>
+      </c>
+      <c r="P26">
+        <v>1</v>
+      </c>
+      <c r="Q26">
+        <v>2</v>
+      </c>
+      <c r="R26" t="s">
+        <v>22</v>
+      </c>
+      <c r="S26">
+        <v>3</v>
+      </c>
+      <c r="T26" t="s">
+        <v>22</v>
+      </c>
+      <c r="U26">
+        <v>4</v>
+      </c>
+      <c r="V26" t="s">
+        <v>22</v>
+      </c>
+      <c r="W26" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>